<commit_message>
added new variable to PET delivery
</commit_message>
<xml_diff>
--- a/data-raw/rpackages.xlsx
+++ b/data-raw/rpackages.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="448">
   <si>
     <t xml:space="preserve">Domain</t>
   </si>
@@ -1361,6 +1361,12 @@
   </si>
   <si>
     <t xml:space="preserve">officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DescTools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skimr</t>
   </si>
 </sst>
 </file>
@@ -1474,12 +1480,12 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A401" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A422" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D420" activeCellId="0" sqref="D420"/>
+      <selection pane="bottomLeft" activeCell="D451" activeCellId="0" sqref="D451"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.33"/>
@@ -4605,6 +4611,28 @@
       </c>
       <c r="C450" s="0" t="s">
         <v>445</v>
+      </c>
+    </row>
+    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A451" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B451" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C451" s="0" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A452" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B452" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C452" s="0" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>